<commit_message>
Update results with new runs with new Braidwood ARMA
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_h2PTC_results.xlsx
+++ b/use_cases/LWRS/LWRS_h2PTC_results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7136CA52-765C-7A43-913F-8BC3A400D54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57934D4D-05F1-CC4D-89B6-071D3138D3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37360" yWindow="500" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="36080" yWindow="4140" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="New_fin_param" sheetId="2" r:id="rId1"/>
+    <sheet name="Old_fin_param" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Case</t>
   </si>
@@ -158,6 +159,15 @@
   <si>
     <t>Synfuel Plant Capacity</t>
   </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Plant capacity</t>
+  </si>
+  <si>
+    <t>Synfuel premium</t>
+  </si>
 </sst>
 </file>
 
@@ -166,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,6 +196,14 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -204,19 +222,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -234,6 +255,512 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>New_fin_param!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="59000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="15875">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;?_);_(@_)" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>New_fin_param!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Plant capacity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity price</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Synfuel premium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>New_fin_param!$B$11:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>424020089.92000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1366824354.6199999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1188037661.8399997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DE3-3D43-904F-33E50F18F005}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>New_fin_param!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000">
+                <a:alpha val="78000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="15875">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-9DE3-3D43-904F-33E50F18F005}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;?_);_(@_)" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>New_fin_param!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Plant capacity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity price</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Synfuel premium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>New_fin_param!$C$11:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1474510909.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1757036210.3399997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1762016155.3899999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9DE3-3D43-904F-33E50F18F005}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="300"/>
+        <c:overlap val="100"/>
+        <c:axId val="1079498976"/>
+        <c:axId val="1079459696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1079498976"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1079459696"/>
+        <c:crossesAt val="1474510909"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1079459696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;?_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1079498976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -269,7 +796,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$12</c:f>
+              <c:f>Old_fin_param!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -298,7 +825,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:f>Old_fin_param!$E$13:$E$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -316,7 +843,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:f>Old_fin_param!$D$13:$D$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -345,7 +872,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$13:$A$15</c:f>
+              <c:f>Old_fin_param!$A$13:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -362,7 +889,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$15</c:f>
+              <c:f>Old_fin_param!$B$13:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -389,7 +916,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$12</c:f>
+              <c:f>Old_fin_param!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -418,7 +945,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:f>Old_fin_param!$E$13:$E$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -436,7 +963,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:f>Old_fin_param!$D$13:$D$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -465,7 +992,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$13:$A$15</c:f>
+              <c:f>Old_fin_param!$A$13:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -482,7 +1009,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$13:$C$15</c:f>
+              <c:f>Old_fin_param!$C$13:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -707,7 +1234,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -733,7 +1260,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Old_fin_param!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -762,7 +1289,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:f>Old_fin_param!$F$3:$F$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -777,7 +1304,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:f>Old_fin_param!$F$3:$F$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -803,7 +1330,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$4</c:f>
+              <c:f>Old_fin_param!$A$3:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -817,7 +1344,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$4</c:f>
+              <c:f>Old_fin_param!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1109,7 +1636,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1212,7 +1739,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:f>Old_fin_param!$D$13:$D$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1230,7 +1757,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:f>Old_fin_param!$D$13:$D$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1262,7 +1789,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Q$33:$Q$35</c:f>
+              <c:f>Old_fin_param!$Q$33:$Q$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1279,7 +1806,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$33:$R$35</c:f>
+              <c:f>Old_fin_param!$R$33:$R$35</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1383,7 +1910,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:f>Old_fin_param!$E$13:$E$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1401,7 +1928,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:f>Old_fin_param!$E$13:$E$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1433,7 +1960,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Q$33:$Q$35</c:f>
+              <c:f>Old_fin_param!$Q$33:$Q$35</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1450,7 +1977,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$33:$S$35</c:f>
+              <c:f>Old_fin_param!$S$33:$S$35</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1794,8 +2321,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2300,7 +2867,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2504,22 +3071,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2624,8 +3192,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2757,19 +3325,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2803,7 +3372,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3007,6 +3576,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -3308,6 +4380,362 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3CDDCEE-4833-6DCC-7A26-E381CF5B1F73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.54863</cdr:x>
+      <cdr:y>0.01943</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.83825</cdr:x>
+      <cdr:y>0.06286</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CB80F9F-6919-B9CE-5CCD-98C3DD19EDE7}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6375400" y="107950"/>
+          <a:ext cx="3365500" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Reference case Δ(NPV)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> = $1,474,510,909</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.0153</cdr:x>
+      <cdr:y>0.30743</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.15847</cdr:x>
+      <cdr:y>0.36229</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB77387C-CA14-B6CC-C560-5ED6EDF07A7F}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="177800" y="1708150"/>
+          <a:ext cx="1663700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[400, 1000] MWe </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00107</cdr:x>
+      <cdr:y>0.58286</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.15632</cdr:x>
+      <cdr:y>0.65029</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26AA5548-A60A-D05C-0D51-011C1B561077}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="12701" y="3238500"/>
+          <a:ext cx="1841500" cy="374650"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[23, LMP, 65] $/MWe </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.01202</cdr:x>
+      <cdr:y>0.85486</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.15519</cdr:x>
+      <cdr:y>0.90971</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26AA5548-A60A-D05C-0D51-011C1B561077}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="139700" y="4749800"/>
+          <a:ext cx="1663700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[x0.8, x1, x1.2] </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3716,11 +5144,312 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D006ED-368F-3443-97DC-C381FA958F9D}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2163277142.8400002</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11351425.8906</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2/B2</f>
+        <v>5.2473285395590067E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3637788051.8800001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1843007.97505</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D8" si="0">C3/B3</f>
+        <v>5.0662873943344163E-4</v>
+      </c>
+      <c r="E3" s="3">
+        <f>B3-$B$2</f>
+        <v>1474510909.04</v>
+      </c>
+      <c r="F3" s="2">
+        <f>SQRT(POWER($C$2,2)+POWER(C3,2))</f>
+        <v>11500067.310493531</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G8" si="1">ABS(F3/E3)</f>
+        <v>7.7992419316726541E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3530101497.46</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.0263049764099996E-7</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4238414901176515E-16</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E8" si="2">B4-$B$2</f>
+        <v>1366824354.6199999</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F8" si="3">SQRT(POWER($C$2,2)+POWER(C4,2))</f>
+        <v>11351425.8906</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>8.3049631448481806E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3920313353.1799998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.0263049764099996E-7</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2821181685216219E-16</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="2"/>
+        <v>1757036210.3399997</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="3"/>
+        <v>11351425.8906</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4605531882597992E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3351314804.6799998</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1615642.4137200001</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8209210649617548E-4</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="2"/>
+        <v>1188037661.8399997</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="3"/>
+        <v>11465826.187361946</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6510628876899356E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3925293298.23</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1845230.25819</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>4.7008723119417708E-4</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
+        <v>1762016155.3899999</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>11500423.66417533</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5268548355788807E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2587297232.7600002</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6695678.8247600002</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5879047602185941E-3</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
+        <v>424020089.92000008</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>13179035.80214135</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1081158924870376E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3">
+        <f>E8</f>
+        <v>424020089.92000008</v>
+      </c>
+      <c r="C11" s="2">
+        <f>E3</f>
+        <v>1474510909.04</v>
+      </c>
+      <c r="D11" s="3">
+        <f>F8</f>
+        <v>13179035.80214135</v>
+      </c>
+      <c r="E11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3">
+        <f>E4</f>
+        <v>1366824354.6199999</v>
+      </c>
+      <c r="C12" s="3">
+        <f>E5</f>
+        <v>1757036210.3399997</v>
+      </c>
+      <c r="D12" s="3">
+        <f>F4</f>
+        <v>11351425.8906</v>
+      </c>
+      <c r="E12" s="3">
+        <f>F5</f>
+        <v>11351425.8906</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3">
+        <f>E6</f>
+        <v>1188037661.8399997</v>
+      </c>
+      <c r="C13" s="3">
+        <f>E7</f>
+        <v>1762016155.3899999</v>
+      </c>
+      <c r="D13" s="3">
+        <f>F6</f>
+        <v>11465826.187361946</v>
+      </c>
+      <c r="E13" s="3">
+        <f>F7</f>
+        <v>11500423.66417533</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3733,8 +5462,9 @@
     <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" customWidth="1"/>
     <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -4097,7 +5827,7 @@
       </c>
     </row>
     <row r="29" spans="17:19" x14ac:dyDescent="0.2">
-      <c r="Q29" t="s">
+      <c r="Q29" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4149,7 +5879,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q29" r:id="rId1" xr:uid="{AA26A45C-2C3B-4E4D-BAD6-FE9E618B6ABB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest results with periodic cycle for electricity prices
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_h2PTC_results.xlsx
+++ b/use_cases/LWRS/LWRS_h2PTC_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57934D4D-05F1-CC4D-89B6-071D3138D3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF3DE14-BC4D-234E-A3A2-C86760991D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36080" yWindow="4140" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="35840" yWindow="1800" windowWidth="38400" windowHeight="24000" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="New_fin_param" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Case</t>
   </si>
@@ -163,10 +163,19 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Plant capacity</t>
+    <t>Synfuel Price Premium</t>
   </si>
   <si>
-    <t>Synfuel premium</t>
+    <t>Without H₂ PTC</t>
+  </si>
+  <si>
+    <t>co2_low</t>
+  </si>
+  <si>
+    <t>co2_high</t>
+  </si>
+  <si>
+    <t>CO2 Cost</t>
   </si>
 </sst>
 </file>
@@ -280,7 +289,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>New_fin_param!$B$10</c:f>
+              <c:f>New_fin_param!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -300,7 +309,24 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:glow>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="contrasting" dir="t">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d prstMaterial="metal">
+              <a:bevelT w="19050" prst="artDeco"/>
+              <a:bevelB w="19050" prst="artDeco"/>
+            </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -362,37 +388,94 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>New_fin_param!$D$14:$D$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>13044061.337726347</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14584955.770416418</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>New_fin_param!$D$14:$D$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>13044061.337726347</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14584955.770416418</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>New_fin_param!$A$11:$A$13</c:f>
+              <c:f>New_fin_param!$A$14:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Plant capacity</c:v>
+                  <c:v>Synfuel Plant Capacity</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Electricity price</c:v>
+                  <c:v>Synfuel Price Premium</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Synfuel premium</c:v>
+                  <c:v>Electricity Price</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CO2 Cost</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>New_fin_param!$B$11:$B$13</c:f>
+              <c:f>New_fin_param!$B$14:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>424020089.92000008</c:v>
+                  <c:v>218407032.44999981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1366824354.6199999</c:v>
+                  <c:v>1142948852.8099999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1188037661.8399997</c:v>
+                  <c:v>1366824354.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1430606193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,7 +491,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>New_fin_param!$C$10</c:f>
+              <c:f>New_fin_param!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -423,12 +506,17 @@
                 <a:alpha val="78000"/>
               </a:srgbClr>
             </a:solidFill>
-            <a:ln w="15875">
+            <a:ln w="15875" cap="flat">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="dkEdge"/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -500,37 +588,94 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>New_fin_param!$E$14:$E$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14749672.60467495</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>New_fin_param!$E$14:$E$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14749672.60467495</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>New_fin_param!$A$11:$A$13</c:f>
+              <c:f>New_fin_param!$A$14:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Plant capacity</c:v>
+                  <c:v>Synfuel Plant Capacity</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Electricity price</c:v>
+                  <c:v>Synfuel Price Premium</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Synfuel premium</c:v>
+                  <c:v>Electricity Price</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CO2 Cost</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>New_fin_param!$C$11:$C$13</c:f>
+              <c:f>New_fin_param!$C$14:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1474510909.04</c:v>
+                  <c:v>1430198349.0599999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1757036210.3399997</c:v>
+                  <c:v>1716954264.23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1762016155.3899999</c:v>
+                  <c:v>1757036210.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1432311825.9200001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,7 +742,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1079459696"/>
-        <c:crossesAt val="1474510909"/>
+        <c:crossesAt val="1430198349.0599999"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -761,6 +906,374 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>New_fin_param!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>11425359.402747918</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11493899.482378878</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>New_fin_param!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>11425359.402747918</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11493899.482378878</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>New_fin_param!$A$3:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Without H₂ PTC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>New_fin_param!$E$3:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-1425565019.6010003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1430198349.0599999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE0E-BF45-8A6C-910CE58DBBFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="636359968"/>
+        <c:axId val="884955680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="636359968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="884955680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="884955680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Δ(NPV)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;?_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="636359968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1234,7 +1747,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1636,7 +2149,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2242,13 +2755,10 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -2361,6 +2871,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -2867,7 +3417,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3071,23 +3621,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3192,8 +3741,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3325,20 +3874,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3372,7 +3920,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3576,22 +4124,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3696,8 +4245,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3829,19 +4378,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3875,7 +4425,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4079,6 +4629,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -4383,16 +5436,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4412,6 +5465,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>162277</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>187677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>437445</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B51A2334-4BBE-D99A-2FD6-8896312AC55C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4457,7 +5546,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+            <a:rPr lang="en-US" sz="1400" b="1">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -4465,14 +5554,14 @@
             <a:t>Reference case Δ(NPV)</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> = $1,474,510,909</a:t>
+            <a:t> = $1,430,198,349</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
             <a:solidFill>
               <a:srgbClr val="C00000"/>
             </a:solidFill>
@@ -4483,12 +5572,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0153</cdr:x>
-      <cdr:y>0.30743</cdr:y>
+      <cdr:x>0.01705</cdr:x>
+      <cdr:y>0.27509</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.15847</cdr:x>
-      <cdr:y>0.36229</cdr:y>
+      <cdr:x>0.19372</cdr:x>
+      <cdr:y>0.32995</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4503,8 +5592,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="177800" y="1708150"/>
-          <a:ext cx="1663700" cy="304800"/>
+          <a:off x="216261" y="1484980"/>
+          <a:ext cx="2241466" cy="296146"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4516,7 +5605,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1400"/>
-            <a:t>[400, 1000] MWe </a:t>
+            <a:t>[400, 1000, N/A] MWe </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4524,12 +5613,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.00107</cdr:x>
-      <cdr:y>0.58286</cdr:y>
+      <cdr:x>0.02232</cdr:x>
+      <cdr:y>0.6905</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.15632</cdr:x>
-      <cdr:y>0.65029</cdr:y>
+      <cdr:x>0.17757</cdr:x>
+      <cdr:y>0.75793</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4544,8 +5633,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="12701" y="3238500"/>
-          <a:ext cx="1841500" cy="374650"/>
+          <a:off x="283195" y="3727459"/>
+          <a:ext cx="1969703" cy="364002"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4629,12 +5718,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.01202</cdr:x>
-      <cdr:y>0.85486</cdr:y>
+      <cdr:x>0.06185</cdr:x>
+      <cdr:y>0.48746</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.15519</cdr:x>
-      <cdr:y>0.90971</cdr:y>
+      <cdr:x>0.17529</cdr:x>
+      <cdr:y>0.5526</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4649,8 +5738,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="139700" y="4749800"/>
-          <a:ext cx="1663700" cy="304800"/>
+          <a:off x="784668" y="2631393"/>
+          <a:ext cx="1439247" cy="351639"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4727,6 +5816,111 @@
           <a:r>
             <a:rPr lang="en-US" sz="1400"/>
             <a:t>[x0.8, x1, x1.2] </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02402</cdr:x>
+      <cdr:y>0.89034</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.17927</cdr:x>
+      <cdr:y>0.95777</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1077D5F8-C748-21F0-1680-A2B87A7E2AB9}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="304800" y="4806244"/>
+          <a:ext cx="1969703" cy="364002"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[1, Supply, 75] $/ton </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5145,18 +6339,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D006ED-368F-3443-97DC-C381FA958F9D}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -5188,10 +6383,10 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>2163277142.8400002</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>11351425.8906</v>
       </c>
       <c r="D2" s="1">
@@ -5201,242 +6396,343 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3637788051.8800001</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1843007.97505</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D8" si="0">C3/B3</f>
-        <v>5.0662873943344163E-4</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B3" s="3">
+        <v>737712123.23899996</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1297677.8229499999</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="3">
         <f>B3-$B$2</f>
-        <v>1474510909.04</v>
+        <v>-1425565019.6010003</v>
       </c>
       <c r="F3" s="2">
         <f>SQRT(POWER($C$2,2)+POWER(C3,2))</f>
-        <v>11500067.310493531</v>
-      </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G8" si="1">ABS(F3/E3)</f>
-        <v>7.7992419316726541E-3</v>
+        <v>11425359.402747918</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3530101497.46</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5.0263049764099996E-7</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3593475491.9000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1804121.8255</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>1.4238414901176515E-16</v>
+        <f t="shared" ref="D4:D11" si="0">C4/B4</f>
+        <v>5.0205485735651861E-4</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E8" si="2">B4-$B$2</f>
-        <v>1366824354.6199999</v>
+        <f>B4-$B$2</f>
+        <v>1430198349.0599999</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ref="F4:F8" si="3">SQRT(POWER($C$2,2)+POWER(C4,2))</f>
-        <v>11351425.8906</v>
+        <f>SQRT(POWER($C$2,2)+POWER(C4,2))</f>
+        <v>11493899.482378878</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>8.3049631448481806E-3</v>
+        <f t="shared" ref="G4:G11" si="1">ABS(F4/E4)</f>
+        <v>8.036577227161017E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3920313353.1799998</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5.0263049764099996E-7</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3530101497.3600001</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5.3312014996999996E-7</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>1.2821181685216219E-16</v>
+        <v>1.5102119595391121E-16</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="2"/>
-        <v>1757036210.3399997</v>
+        <f t="shared" ref="E5:E11" si="2">B5-$B$2</f>
+        <v>1366824354.52</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F5:F11" si="3">SQRT(POWER($C$2,2)+POWER(C5,2))</f>
         <v>11351425.8906</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>6.4605531882597992E-3</v>
+        <v>8.30496314545579E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3351314804.6799998</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1615642.4137200001</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3920313353.0900002</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.3312014996999996E-7</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>4.8209210649617548E-4</v>
+        <v>1.3598916768982086E-16</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="2"/>
-        <v>1188037661.8399997</v>
+        <v>1757036210.25</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="3"/>
-        <v>11465826.187361946</v>
+        <v>11351425.8906</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>9.6510628876899356E-3</v>
+        <v>6.4605531885907246E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3925293298.23</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1845230.25819</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3306225995.6500001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2003974.74498</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>4.7008723119417708E-4</v>
+        <v>6.0612152575674754E-4</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="2"/>
-        <v>1762016155.3899999</v>
+        <f>B7-$B$2</f>
+        <v>1142948852.8099999</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="3"/>
-        <v>11500423.66417533</v>
+        <v>11526959.032125587</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>6.5268548355788807E-3</v>
+        <v>1.0085279847637933E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2587297232.7600002</v>
-      </c>
-      <c r="C8" s="2">
-        <v>6695678.8247600002</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3880231407.0700002</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1098631.7476300001</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>2.5879047602185941E-3</v>
+        <v>2.8313562578464552E-4</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="2"/>
-        <v>424020089.92000008</v>
+        <v>1716954264.23</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="3"/>
-        <v>13179035.80214135</v>
+        <v>11404466.733113151</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>3.1081158924870376E-2</v>
+        <v>6.6422658836679587E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2381684175.29</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6425937.0081399996</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6980642835893894E-3</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="2"/>
+        <v>218407032.44999981</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>13044061.337726347</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>5.9723632482907983E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3593883335.8400002</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1936846.0653899999</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3892847496600775E-4</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="2"/>
+        <v>1430606193</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="3"/>
+        <v>11515478.384800205</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>8.0493698693223856E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3">
-        <f>E8</f>
-        <v>424020089.92000008</v>
-      </c>
-      <c r="C11" s="2">
-        <f>E3</f>
-        <v>1474510909.04</v>
-      </c>
-      <c r="D11" s="3">
-        <f>F8</f>
-        <v>13179035.80214135</v>
-      </c>
-      <c r="E11">
-        <f>0</f>
-        <v>0</v>
+        <v>3595588968.7600002</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2731170.3485400002</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>7.5958914444046997E-4</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
+        <v>1432311825.9200001</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>11675365.571258491</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>8.1514132327708665E-3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3">
-        <f>E4</f>
-        <v>1366824354.6199999</v>
-      </c>
-      <c r="C12" s="3">
-        <f>E5</f>
-        <v>1757036210.3399997</v>
-      </c>
-      <c r="D12" s="3">
-        <f>F4</f>
-        <v>11351425.8906</v>
-      </c>
-      <c r="E12" s="3">
-        <f>F5</f>
-        <v>11351425.8906</v>
-      </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3">
+        <f>E9</f>
+        <v>218407032.44999981</v>
+      </c>
+      <c r="C14" s="2">
+        <f>E4</f>
+        <v>1430198349.0599999</v>
+      </c>
+      <c r="D14" s="3">
+        <f>F9</f>
+        <v>13044061.337726347</v>
+      </c>
+      <c r="E14">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3">
+        <f>E7</f>
+        <v>1142948852.8099999</v>
+      </c>
+      <c r="C15" s="3">
+        <f>E8</f>
+        <v>1716954264.23</v>
+      </c>
+      <c r="D15" s="3">
+        <v>14584955.770416418</v>
+      </c>
+      <c r="E15" s="3">
+        <v>14749672.60467495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3">
+        <f>E5</f>
+        <v>1366824354.52</v>
+      </c>
+      <c r="C16" s="3">
         <f>E6</f>
-        <v>1188037661.8399997</v>
-      </c>
-      <c r="C13" s="3">
-        <f>E7</f>
-        <v>1762016155.3899999</v>
-      </c>
-      <c r="D13" s="3">
-        <f>F6</f>
-        <v>11465826.187361946</v>
-      </c>
-      <c r="E13" s="3">
-        <f>F7</f>
-        <v>11500423.66417533</v>
-      </c>
+        <v>1757036210.25</v>
+      </c>
+      <c r="D16" s="3">
+        <v>14477794.612199999</v>
+      </c>
+      <c r="E16" s="3">
+        <v>14477794.612199999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3">
+        <f>E10</f>
+        <v>1430606193</v>
+      </c>
+      <c r="C17" s="3">
+        <f>E11</f>
+        <v>1432311825.9200001</v>
+      </c>
+      <c r="D17" s="3">
+        <v>14794850.990930472</v>
+      </c>
+      <c r="E17" s="3">
+        <v>14612923.893369727</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>